<commit_message>
Site updated: 2019-12-09 19:01:10
</commit_message>
<xml_diff>
--- a/2019/12/04/接口工具Postman的学习使用/GO桌面团队测试人员2019Q3Q4_dKPI表格.xlsx
+++ b/2019/12/04/接口工具Postman的学习使用/GO桌面团队测试人员2019Q3Q4_dKPI表格.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcy/Documents/NewBlog/public/2019/12/04/接口工具Postman的学习使用/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B500882E-84D2-6D40-B28D-F239C85BE2A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA7C9AF-5631-1E40-8477-E98A64EA6144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="24700" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24700" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>指标分类</t>
   </si>
@@ -55,6 +55,585 @@
     <t>60%</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>此指标主要衡量团队推动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">修复的能力
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>修复率</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>（修复的有效</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>有效</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>总数）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">x100%
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>有效</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>：解决情况为未解决、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="_GBK;方"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Fixed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Incomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Cannot Reproduce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Keep
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>无效</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>：解决情况为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Won’t Fix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Duplicate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>修复</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>：状态为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Resolved</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Closed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>未修复</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>：状态为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>In Progress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Reopened
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>大家在完成情况里面备注注明自己实际的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>修复率</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">此指标主要衡量团队所负责产品的测试质量
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">一次性发包成功率 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">（未补包的包数量 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>总共发布的包数量）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">x100%
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>：主题、壁纸、语言包等不计入包数量；一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>VC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">计为一个包
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>只统计由测试人员漏测导致的补包：如必现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>crash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">，基本功能异常
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>这些情况不计为测试人员补包：如非必现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>crash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t xml:space="preserve">、需求插入、留存数据调整
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+      </rPr>
+      <t>大家在完成情况里面注明自己实际的发包数、补包数；数据客观填写</t>
+    </r>
+  </si>
+  <si>
     <t>此指标主要衡量测试团队的测试规范性
 客观进行自评</t>
   </si>
@@ -1412,1012 +1991,12 @@
     </r>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>此指标主要衡量团队推动</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">修复的能力
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>修复率</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（修复的有效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>有效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>总数）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">x100%
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>有效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：解决情况为未解决、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="_GBK;方"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Fixed</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Incomplete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Cannot Reproduce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Keep
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>无效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：解决情况为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Won’t Fix</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Duplicate
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>修复</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：状态为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Resolved</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Closed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>未修复</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：状态为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Open</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>In Progress</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Reopened
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>大家在完成情况里面备注注明自己实际的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>修复率</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>针对</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Palm_Secret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>项目设计了</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>UI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>自动化回归测试，并持续集成在</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Jenkins</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>上，每日对</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>APP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>自动进行回归测试，保证产品质量的稳定性，提示软件可信任度，并以邮件形式发送测试报告。</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>暂时没有开展相关的测试经验及技术的分享</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>修复的有效bug：58</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>有效的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>bug</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>总数：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>修复率：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>58/60 = 0.96</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>在测试执行前，参考需求文档，对其需求功能编写测试用例，并且及时上传</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>SVN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，测试执行后，在测试用例后记录实际的测试结果，并更新</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>SVN</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>发现服务器异常导致多个产品统计获取异常的问题，并及时与服务器反馈，未记录</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>wiki</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">此指标主要衡量团队所负责产品的测试质量
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>一次性发包成功率</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（未补包的包数量</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">/ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>总共发布的包数量）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>x100%
-PS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：主题、壁纸、语言包等不计入包数量；一个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>VC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>计为一个包
-只统计由测试人员漏测导致的补包：如必现</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>crash</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，基本功能异常
-这些情况不计为测试人员补包：如非必现</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>crash</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、需求插入、留存数据调整
-大家在完成情况里面注明自己实际的发包数、补包数；数据客观填写</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>总发包数：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">18
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>未补包数：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>一次性发包成功率：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>16/18 = 0.88</t>
-    </r>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>3</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>创新表现</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>团队精神</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>工作品质</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>工作态度</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>乐于学习新技术并使用在工作中，编写自动化测试脚本用于项目软件回归测试，使用python编写，测试框架采用了pytest以及自动化工具appium，最后集成与Jenkins并使用allure输出测试报告并以邮件形式发送给组内成员。</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>将团队目标作为主目标，积极协助研发发现并解决问题，与运营一起分析数据并给出相关性意见，与产品一同沟通产品的用户体验度以及功能的适用度等。</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次都能保证产品在规定时间内测试质量，有时在保证质量的情况下做到提前发包完成工作，在工作中引入新技术对质量进行保证。</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>自我管理比较严格，偶有迟到，从无早退，请假现象，在工作中投入度比较高，在工作中对于质量保证以及把控进行思考，并用于尝试新方法去保证软件产品的质量</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2537,47 +2116,6 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2793,7 +2331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2821,15 +2359,30 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2851,6 +2404,9 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2869,6 +2425,24 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2888,48 +2462,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4094,9 +3626,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1"/>
@@ -4151,542 +3683,494 @@
       <c r="B2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>22</v>
+      <c r="C2" s="37" t="s">
+        <v>24</v>
       </c>
       <c r="D2" s="6">
         <v>10</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>24</v>
+      <c r="E2" s="38" t="s">
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="132" customHeight="1">
       <c r="A3" s="35"/>
       <c r="B3" s="32"/>
-      <c r="C3" s="27" t="s">
-        <v>25</v>
+      <c r="C3" s="39" t="s">
+        <v>27</v>
       </c>
       <c r="D3" s="6">
         <v>15</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="9"/>
+      <c r="E3" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="126" customHeight="1">
       <c r="A4" s="36"/>
       <c r="B4" s="32"/>
-      <c r="C4" s="27" t="s">
-        <v>28</v>
+      <c r="C4" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="D4" s="6">
         <v>8</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="13"/>
+      <c r="E4" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" ht="203" customHeight="1">
-      <c r="A5" s="14" t="s">
-        <v>12</v>
+      <c r="A5" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="D5" s="6">
         <v>15</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="15"/>
+      <c r="E5" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" ht="148" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="18">
-        <v>2</v>
-      </c>
-      <c r="H6" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="15"/>
+      <c r="D6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" ht="102.75" customHeight="1">
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
-      <c r="C7" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="C7" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="18">
-        <v>2</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="D7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="15"/>
+      <c r="E7" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10" ht="96" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+    <row r="8" spans="1:10" ht="66.5" customHeight="1">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" ht="91" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="15"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="57.25" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="1:10" ht="63" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="23">
-        <v>4</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+    <row r="11" spans="1:10" ht="16" customHeight="1">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="16" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="16" customHeight="1">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="16" customHeight="1">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="16" customHeight="1">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>